<commit_message>
Actualizar el proyecto para la IA
</commit_message>
<xml_diff>
--- a/data/output/Resumen_Pedidos_CONSOLIDADO_09022026.xlsx
+++ b/data/output/Resumen_Pedidos_CONSOLIDADO_09022026.xlsx
@@ -587,40 +587,40 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>2625</v>
+        <v>1085</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>2147</v>
+        <v>865</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>2254</v>
+        <v>908</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>2254</v>
+        <v>908</v>
       </c>
       <c r="G3" s="5" t="n">
         <v>5</v>
       </c>
       <c r="H3" s="3" t="n">
-        <v>828</v>
+        <v>303</v>
       </c>
       <c r="I3" s="3" t="n">
-        <v>92</v>
+        <v>56</v>
       </c>
       <c r="J3" s="4" t="n">
-        <v>2255</v>
+        <v>915</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>105.1</v>
+        <v>105.7</v>
       </c>
       <c r="L3" s="3" t="n">
-        <v>55</v>
+        <v>34</v>
       </c>
       <c r="M3" s="3" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="N3" s="3" t="n">
         <v>2</v>
@@ -632,7 +632,7 @@
         <v>30</v>
       </c>
       <c r="Q3" s="4" t="n">
-        <v>227</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4">
@@ -642,43 +642,43 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" s="4" t="n">
-        <v>1771</v>
+        <v>1387</v>
       </c>
       <c r="D4" s="4" t="n">
-        <v>1649</v>
+        <v>1473</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>1731</v>
+        <v>1547</v>
       </c>
       <c r="F4" s="4" t="n">
-        <v>1731</v>
+        <v>1547</v>
       </c>
       <c r="G4" s="5" t="n">
         <v>5</v>
       </c>
       <c r="H4" s="3" t="n">
-        <v>268</v>
+        <v>322</v>
       </c>
       <c r="I4" s="3" t="n">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="J4" s="4" t="n">
-        <v>1741</v>
+        <v>1565</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>105.6</v>
+        <v>106.2</v>
       </c>
       <c r="L4" s="3" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M4" s="3" t="n">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="N4" s="3" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="O4" s="5" t="n">
         <v>0</v>
@@ -687,7 +687,7 @@
         <v>30</v>
       </c>
       <c r="Q4" s="4" t="n">
-        <v>102</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5">
@@ -697,43 +697,43 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5" s="4" t="n">
-        <v>270</v>
+        <v>157</v>
       </c>
       <c r="D5" s="4" t="n">
-        <v>313</v>
+        <v>167</v>
       </c>
       <c r="E5" s="4" t="n">
-        <v>328</v>
+        <v>176</v>
       </c>
       <c r="F5" s="4" t="n">
-        <v>328</v>
+        <v>176</v>
       </c>
       <c r="G5" s="5" t="n">
         <v>5</v>
       </c>
       <c r="H5" s="3" t="n">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="I5" s="3" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="J5" s="4" t="n">
-        <v>329</v>
+        <v>177</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>105.4</v>
+        <v>105.6</v>
       </c>
       <c r="L5" s="3" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="M5" s="3" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="N5" s="3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="O5" s="5" t="n">
         <v>0</v>
@@ -742,7 +742,7 @@
         <v>30</v>
       </c>
       <c r="Q5" s="4" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6">
@@ -752,43 +752,43 @@
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="4" t="n">
-        <v>1342</v>
+        <v>1211</v>
       </c>
       <c r="D6" s="4" t="n">
-        <v>849</v>
+        <v>780</v>
       </c>
       <c r="E6" s="4" t="n">
-        <v>891</v>
+        <v>819</v>
       </c>
       <c r="F6" s="4" t="n">
-        <v>891</v>
+        <v>819</v>
       </c>
       <c r="G6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="H6" s="3" t="n">
-        <v>238</v>
+        <v>274</v>
       </c>
       <c r="I6" s="3" t="n">
         <v>35</v>
       </c>
       <c r="J6" s="4" t="n">
-        <v>931</v>
+        <v>821</v>
       </c>
       <c r="K6" s="5" t="n">
-        <v>109.7</v>
+        <v>105.3</v>
       </c>
       <c r="L6" s="3" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M6" s="3" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="N6" s="3" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="O6" s="5" t="n">
         <v>0</v>
@@ -797,7 +797,7 @@
         <v>30</v>
       </c>
       <c r="Q6" s="4" t="n">
-        <v>68</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7">
@@ -807,43 +807,43 @@
         </is>
       </c>
       <c r="B7" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C7" s="4" t="n">
-        <v>5742</v>
+        <v>7207</v>
       </c>
       <c r="D7" s="4" t="n">
-        <v>5433</v>
+        <v>5865</v>
       </c>
       <c r="E7" s="4" t="n">
-        <v>5704</v>
+        <v>6158</v>
       </c>
       <c r="F7" s="4" t="n">
-        <v>5704</v>
+        <v>6158</v>
       </c>
       <c r="G7" s="5" t="n">
         <v>5</v>
       </c>
       <c r="H7" s="3" t="n">
-        <v>684</v>
+        <v>670</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="J7" s="4" t="n">
-        <v>5725</v>
+        <v>6184</v>
       </c>
       <c r="K7" s="5" t="n">
         <v>105.4</v>
       </c>
       <c r="L7" s="3" t="n">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="M7" s="3" t="n">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="N7" s="3" t="n">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="O7" s="5" t="n">
         <v>0</v>
@@ -852,7 +852,7 @@
         <v>30</v>
       </c>
       <c r="Q7" s="4" t="n">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8">
@@ -862,43 +862,43 @@
         </is>
       </c>
       <c r="B8" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C8" s="4" t="n">
-        <v>2478</v>
+        <v>2218</v>
       </c>
       <c r="D8" s="4" t="n">
-        <v>2359</v>
+        <v>1563</v>
       </c>
       <c r="E8" s="4" t="n">
-        <v>2477</v>
+        <v>1642</v>
       </c>
       <c r="F8" s="4" t="n">
-        <v>2477</v>
+        <v>1642</v>
       </c>
       <c r="G8" s="5" t="n">
         <v>5</v>
       </c>
       <c r="H8" s="3" t="n">
-        <v>457</v>
+        <v>281</v>
       </c>
       <c r="I8" s="3" t="n">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="J8" s="4" t="n">
-        <v>2481</v>
+        <v>1650</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>105.2</v>
+        <v>105.5</v>
       </c>
       <c r="L8" s="3" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M8" s="3" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="N8" s="3" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="O8" s="5" t="n">
         <v>0</v>
@@ -907,7 +907,7 @@
         <v>30</v>
       </c>
       <c r="Q8" s="4" t="n">
-        <v>137</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9">
@@ -917,40 +917,40 @@
         </is>
       </c>
       <c r="B9" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="4" t="n">
-        <v>1856</v>
+        <v>543</v>
       </c>
       <c r="D9" s="4" t="n">
-        <v>1062</v>
+        <v>549</v>
       </c>
       <c r="E9" s="4" t="n">
-        <v>1116</v>
+        <v>576</v>
       </c>
       <c r="F9" s="4" t="n">
-        <v>1116</v>
+        <v>576</v>
       </c>
       <c r="G9" s="5" t="n">
         <v>5</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>156</v>
+        <v>97</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="J9" s="4" t="n">
-        <v>1123</v>
+        <v>581</v>
       </c>
       <c r="K9" s="5" t="n">
-        <v>105.6</v>
+        <v>105.8</v>
       </c>
       <c r="L9" s="3" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="M9" s="3" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="N9" s="3" t="n">
         <v>0</v>
@@ -962,7 +962,7 @@
         <v>30</v>
       </c>
       <c r="Q9" s="4" t="n">
-        <v>54</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10">
@@ -972,43 +972,43 @@
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C10" s="4" t="n">
-        <v>3184</v>
+        <v>1411</v>
       </c>
       <c r="D10" s="4" t="n">
-        <v>2412</v>
+        <v>1495</v>
       </c>
       <c r="E10" s="4" t="n">
-        <v>2533</v>
+        <v>1570</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>2533</v>
+        <v>1570</v>
       </c>
       <c r="G10" s="5" t="n">
         <v>5</v>
       </c>
       <c r="H10" s="3" t="n">
-        <v>201</v>
+        <v>138</v>
       </c>
       <c r="I10" s="3" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="J10" s="4" t="n">
-        <v>2554</v>
+        <v>1582</v>
       </c>
       <c r="K10" s="5" t="n">
-        <v>105.9</v>
+        <v>105.8</v>
       </c>
       <c r="L10" s="3" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="M10" s="3" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="N10" s="3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O10" s="5" t="n">
         <v>0</v>
@@ -1017,7 +1017,7 @@
         <v>30</v>
       </c>
       <c r="Q10" s="4" t="n">
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11">
@@ -1027,43 +1027,43 @@
         </is>
       </c>
       <c r="B11" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C11" s="4" t="n">
-        <v>342</v>
+        <v>263</v>
       </c>
       <c r="D11" s="4" t="n">
-        <v>409</v>
+        <v>267</v>
       </c>
       <c r="E11" s="4" t="n">
-        <v>429</v>
+        <v>281</v>
       </c>
       <c r="F11" s="4" t="n">
-        <v>429</v>
+        <v>281</v>
       </c>
       <c r="G11" s="5" t="n">
         <v>5</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>109</v>
+        <v>51</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="J11" s="4" t="n">
-        <v>432</v>
+        <v>309</v>
       </c>
       <c r="K11" s="5" t="n">
-        <v>105.7</v>
+        <v>115.4</v>
       </c>
       <c r="L11" s="3" t="n">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="M11" s="3" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="N11" s="3" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="O11" s="5" t="n">
         <v>0</v>
@@ -1072,7 +1072,7 @@
         <v>30</v>
       </c>
       <c r="Q11" s="4" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
@@ -1082,31 +1082,31 @@
         </is>
       </c>
       <c r="B12" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C12" s="4" t="n">
-        <v>2222</v>
+        <v>1282</v>
       </c>
       <c r="D12" s="4" t="n">
-        <v>2078</v>
+        <v>1155</v>
       </c>
       <c r="E12" s="4" t="n">
-        <v>2182</v>
+        <v>1213</v>
       </c>
       <c r="F12" s="4" t="n">
-        <v>2182</v>
+        <v>1213</v>
       </c>
       <c r="G12" s="5" t="n">
         <v>5</v>
       </c>
       <c r="H12" s="3" t="n">
-        <v>348</v>
+        <v>192</v>
       </c>
       <c r="I12" s="3" t="n">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="J12" s="4" t="n">
-        <v>2188</v>
+        <v>1216</v>
       </c>
       <c r="K12" s="5" t="n">
         <v>105.3</v>
@@ -1118,7 +1118,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="3" t="n">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="O12" s="5" t="n">
         <v>0</v>
@@ -1127,7 +1127,7 @@
         <v>30</v>
       </c>
       <c r="Q12" s="4" t="n">
-        <v>99</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13">
@@ -1137,43 +1137,43 @@
         </is>
       </c>
       <c r="B13" s="3" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C13" s="4" t="n">
-        <v>1939</v>
+        <v>2674</v>
       </c>
       <c r="D13" s="4" t="n">
-        <v>1604</v>
+        <v>1301</v>
       </c>
       <c r="E13" s="4" t="n">
-        <v>1684</v>
+        <v>1367</v>
       </c>
       <c r="F13" s="4" t="n">
-        <v>1684</v>
+        <v>1367</v>
       </c>
       <c r="G13" s="5" t="n">
         <v>5</v>
       </c>
       <c r="H13" s="3" t="n">
-        <v>281</v>
+        <v>103</v>
       </c>
       <c r="I13" s="3" t="n">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="J13" s="4" t="n">
-        <v>1687</v>
+        <v>1387</v>
       </c>
       <c r="K13" s="5" t="n">
-        <v>105.2</v>
+        <v>106.6</v>
       </c>
       <c r="L13" s="3" t="n">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="M13" s="3" t="n">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="N13" s="3" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="O13" s="5" t="n">
         <v>0</v>
@@ -1182,7 +1182,7 @@
         <v>30</v>
       </c>
       <c r="Q13" s="4" t="n">
-        <v>106</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>